<commit_message>
Add Todo section to the README doc
</commit_message>
<xml_diff>
--- a/MD Extraction file.xlsx
+++ b/MD Extraction file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdulqadir Abuharrus\Documents\My projects\Dalia PDF Scrape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67B8CD1-D2B0-4E85-B31C-809D06195F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FB4B1E-2CED-453E-8C63-4F09C075C31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="19416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="92">
   <si>
     <t>Headers</t>
   </si>
@@ -2377,16 +2377,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2693,1027 +2687,1527 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="65.44140625" defaultRowHeight="32.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="65.44140625" customWidth="1"/>
+    <col min="3" max="3" width="71.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2">
-        <v>2</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2">
-        <v>2</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2">
-        <v>2</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2">
-        <v>2</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2">
-        <v>2</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2">
-        <v>2</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2">
-        <v>2</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="2">
-        <v>2</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="2">
-        <v>2</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="2">
-        <v>2</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="2">
-        <v>2</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="2">
-        <v>2</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="2">
-        <v>2</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="2">
-        <v>2</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="2">
-        <v>2</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="2">
-        <v>2</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="2">
-        <v>2</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="2">
-        <v>2</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28">
         <v>3</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29">
         <v>3</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="2">
-        <v>2</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="2">
-        <v>2</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="2">
-        <v>2</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="2">
-        <v>2</v>
-      </c>
-      <c r="C33" s="4" t="s">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="2">
-        <v>2</v>
-      </c>
-      <c r="C34" s="4" t="s">
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="2">
-        <v>2</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="2">
-        <v>2</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="2">
-        <v>2</v>
-      </c>
-      <c r="C37" s="4" t="s">
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="2">
-        <v>2</v>
-      </c>
-      <c r="C38" s="4" t="s">
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="2">
-        <v>2</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="2">
-        <v>2</v>
-      </c>
-      <c r="C40" s="4" t="s">
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="2">
-        <v>2</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>80</v>
       </c>
-      <c r="B42" s="2">
-        <v>2</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>82</v>
       </c>
-      <c r="B43" s="2">
-        <v>2</v>
-      </c>
-      <c r="C43" s="4" t="s">
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="2">
-        <v>2</v>
-      </c>
-      <c r="C44" s="4" t="s">
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="2">
-        <v>2</v>
-      </c>
-      <c r="C45" s="4" t="s">
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="2">
-        <v>2</v>
-      </c>
-      <c r="C46" s="4" t="s">
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="2">
-        <v>2</v>
-      </c>
-      <c r="C47" s="4" t="s">
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="2">
-        <v>2</v>
-      </c>
-      <c r="C48" s="4" t="s">
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49">
         <v>1</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="2">
-        <v>2</v>
-      </c>
-      <c r="C50" s="4" t="s">
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="2">
-        <v>2</v>
-      </c>
-      <c r="C51" s="4" t="s">
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>11</v>
       </c>
-      <c r="B52" s="2">
-        <v>2</v>
-      </c>
-      <c r="C52" s="4" t="s">
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="2">
-        <v>2</v>
-      </c>
-      <c r="C53" s="4" t="s">
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>15</v>
       </c>
-      <c r="B54" s="2">
-        <v>2</v>
-      </c>
-      <c r="C54" s="4" t="s">
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>18</v>
       </c>
-      <c r="B56" s="2">
-        <v>2</v>
-      </c>
-      <c r="C56" s="4" t="s">
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>20</v>
       </c>
-      <c r="B57" s="2">
-        <v>2</v>
-      </c>
-      <c r="C57" s="4" t="s">
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>22</v>
       </c>
-      <c r="B58" s="2">
-        <v>2</v>
-      </c>
-      <c r="C58" s="4" t="s">
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="2">
-        <v>2</v>
-      </c>
-      <c r="C59" s="4" t="s">
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>26</v>
       </c>
-      <c r="B60" s="2">
-        <v>2</v>
-      </c>
-      <c r="C60" s="4" t="s">
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>28</v>
       </c>
-      <c r="B61" s="2">
-        <v>2</v>
-      </c>
-      <c r="C61" s="4" t="s">
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>30</v>
       </c>
-      <c r="B62" s="2">
-        <v>2</v>
-      </c>
-      <c r="C62" s="4" t="s">
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>32</v>
       </c>
-      <c r="B63" s="2">
-        <v>2</v>
-      </c>
-      <c r="C63" s="4" t="s">
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="2">
-        <v>2</v>
-      </c>
-      <c r="C64" s="4" t="s">
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>36</v>
       </c>
-      <c r="B65" s="2">
-        <v>2</v>
-      </c>
-      <c r="C65" s="4" t="s">
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="2">
-        <v>2</v>
-      </c>
-      <c r="C66" s="4" t="s">
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>40</v>
       </c>
-      <c r="B67" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="216" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>41</v>
       </c>
-      <c r="B68" s="2">
-        <v>2</v>
-      </c>
-      <c r="C68" s="4" t="s">
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>43</v>
       </c>
-      <c r="B69" s="2">
-        <v>2</v>
-      </c>
-      <c r="C69" s="4" t="s">
+      <c r="B69">
+        <v>2</v>
+      </c>
+      <c r="C69" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>45</v>
       </c>
-      <c r="B70" s="2">
-        <v>2</v>
-      </c>
-      <c r="C70" s="4" t="s">
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>47</v>
       </c>
-      <c r="B71" s="2">
-        <v>2</v>
-      </c>
-      <c r="C71" s="4" t="s">
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>49</v>
       </c>
-      <c r="B72" s="2">
-        <v>2</v>
-      </c>
-      <c r="C72" s="4" t="s">
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>51</v>
       </c>
-      <c r="B73" s="2">
-        <v>2</v>
-      </c>
-      <c r="C73" s="4" t="s">
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>53</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74">
         <v>3</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>53</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75">
         <v>3</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C75" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>56</v>
       </c>
-      <c r="B76" s="2">
-        <v>2</v>
-      </c>
-      <c r="C76" s="4" t="s">
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>58</v>
       </c>
-      <c r="B77" s="2">
-        <v>2</v>
-      </c>
-      <c r="C77" s="4" t="s">
+      <c r="B77">
+        <v>2</v>
+      </c>
+      <c r="C77" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>60</v>
       </c>
-      <c r="B78" s="2">
-        <v>2</v>
-      </c>
-      <c r="C78" s="4" t="s">
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>62</v>
       </c>
-      <c r="B79" s="2">
-        <v>2</v>
-      </c>
-      <c r="C79" s="4" t="s">
+      <c r="B79">
+        <v>2</v>
+      </c>
+      <c r="C79" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>64</v>
       </c>
-      <c r="B80" s="2">
-        <v>2</v>
-      </c>
-      <c r="C80" s="4" t="s">
+      <c r="B80">
+        <v>2</v>
+      </c>
+      <c r="C80" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>66</v>
       </c>
-      <c r="B81" s="2">
-        <v>2</v>
-      </c>
-      <c r="C81" s="4" t="s">
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>68</v>
       </c>
-      <c r="B82" s="2">
-        <v>2</v>
-      </c>
-      <c r="C82" s="4" t="s">
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>70</v>
       </c>
-      <c r="B83" s="2">
-        <v>2</v>
-      </c>
-      <c r="C83" s="4" t="s">
+      <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>72</v>
       </c>
-      <c r="B84" s="2">
-        <v>2</v>
-      </c>
-      <c r="C84" s="4" t="s">
+      <c r="B84">
+        <v>2</v>
+      </c>
+      <c r="C84" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="2">
-        <v>2</v>
-      </c>
-      <c r="C85" s="4" t="s">
+      <c r="B85">
+        <v>2</v>
+      </c>
+      <c r="C85" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>76</v>
       </c>
-      <c r="B86" s="2">
-        <v>2</v>
-      </c>
-      <c r="C86" s="4" t="s">
+      <c r="B86">
+        <v>2</v>
+      </c>
+      <c r="C86" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>78</v>
       </c>
-      <c r="B87" s="2">
-        <v>2</v>
-      </c>
-      <c r="C87" s="4" t="s">
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>80</v>
       </c>
-      <c r="B88" s="2">
-        <v>2</v>
-      </c>
-      <c r="C88" s="4" t="s">
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="C88" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>82</v>
       </c>
-      <c r="B89" s="2">
-        <v>2</v>
-      </c>
-      <c r="C89" s="4" t="s">
+      <c r="B89">
+        <v>2</v>
+      </c>
+      <c r="C89" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>84</v>
       </c>
-      <c r="B90" s="2">
-        <v>2</v>
-      </c>
-      <c r="C90" s="4" t="s">
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="C90" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>86</v>
       </c>
-      <c r="B91" s="2">
-        <v>2</v>
-      </c>
-      <c r="C91" s="4" t="s">
+      <c r="B91">
+        <v>2</v>
+      </c>
+      <c r="C91" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>88</v>
       </c>
-      <c r="B92" s="2">
-        <v>2</v>
-      </c>
-      <c r="C92" s="4" t="s">
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>90</v>
       </c>
-      <c r="B93" s="2">
-        <v>2</v>
-      </c>
-      <c r="C93" s="4" t="s">
+      <c r="B93">
+        <v>2</v>
+      </c>
+      <c r="C93" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94">
+        <v>2</v>
+      </c>
+      <c r="C94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>7</v>
+      </c>
+      <c r="B96">
+        <v>2</v>
+      </c>
+      <c r="C96" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>9</v>
+      </c>
+      <c r="B97">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98">
+        <v>2</v>
+      </c>
+      <c r="C98" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>13</v>
+      </c>
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>15</v>
+      </c>
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>17</v>
+      </c>
+      <c r="B101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>18</v>
+      </c>
+      <c r="B102">
+        <v>2</v>
+      </c>
+      <c r="C102" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>22</v>
+      </c>
+      <c r="B104">
+        <v>2</v>
+      </c>
+      <c r="C104" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>24</v>
+      </c>
+      <c r="B105">
+        <v>2</v>
+      </c>
+      <c r="C105" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106">
+        <v>2</v>
+      </c>
+      <c r="C106" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>28</v>
+      </c>
+      <c r="B107">
+        <v>2</v>
+      </c>
+      <c r="C107" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>30</v>
+      </c>
+      <c r="B108">
+        <v>2</v>
+      </c>
+      <c r="C108" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>32</v>
+      </c>
+      <c r="B109">
+        <v>2</v>
+      </c>
+      <c r="C109" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>34</v>
+      </c>
+      <c r="B110">
+        <v>2</v>
+      </c>
+      <c r="C110" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>36</v>
+      </c>
+      <c r="B111">
+        <v>2</v>
+      </c>
+      <c r="C111" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>38</v>
+      </c>
+      <c r="B112">
+        <v>2</v>
+      </c>
+      <c r="C112" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>40</v>
+      </c>
+      <c r="B113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>41</v>
+      </c>
+      <c r="B114">
+        <v>2</v>
+      </c>
+      <c r="C114" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>43</v>
+      </c>
+      <c r="B115">
+        <v>2</v>
+      </c>
+      <c r="C115" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>45</v>
+      </c>
+      <c r="B116">
+        <v>2</v>
+      </c>
+      <c r="C116" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>47</v>
+      </c>
+      <c r="B117">
+        <v>2</v>
+      </c>
+      <c r="C117" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>49</v>
+      </c>
+      <c r="B118">
+        <v>2</v>
+      </c>
+      <c r="C118" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>51</v>
+      </c>
+      <c r="B119">
+        <v>2</v>
+      </c>
+      <c r="C119" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>53</v>
+      </c>
+      <c r="B120">
+        <v>3</v>
+      </c>
+      <c r="C120" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>53</v>
+      </c>
+      <c r="B121">
+        <v>3</v>
+      </c>
+      <c r="C121" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>56</v>
+      </c>
+      <c r="B122">
+        <v>2</v>
+      </c>
+      <c r="C122" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>58</v>
+      </c>
+      <c r="B123">
+        <v>2</v>
+      </c>
+      <c r="C123" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>60</v>
+      </c>
+      <c r="B124">
+        <v>2</v>
+      </c>
+      <c r="C124" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>62</v>
+      </c>
+      <c r="B125">
+        <v>2</v>
+      </c>
+      <c r="C125" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>64</v>
+      </c>
+      <c r="B126">
+        <v>2</v>
+      </c>
+      <c r="C126" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>66</v>
+      </c>
+      <c r="B127">
+        <v>2</v>
+      </c>
+      <c r="C127" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>68</v>
+      </c>
+      <c r="B128">
+        <v>2</v>
+      </c>
+      <c r="C128" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>70</v>
+      </c>
+      <c r="B129">
+        <v>2</v>
+      </c>
+      <c r="C129" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>72</v>
+      </c>
+      <c r="B130">
+        <v>2</v>
+      </c>
+      <c r="C130" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>74</v>
+      </c>
+      <c r="B131">
+        <v>2</v>
+      </c>
+      <c r="C131" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>76</v>
+      </c>
+      <c r="B132">
+        <v>2</v>
+      </c>
+      <c r="C132" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>78</v>
+      </c>
+      <c r="B133">
+        <v>2</v>
+      </c>
+      <c r="C133" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>80</v>
+      </c>
+      <c r="B134">
+        <v>2</v>
+      </c>
+      <c r="C134" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>82</v>
+      </c>
+      <c r="B135">
+        <v>2</v>
+      </c>
+      <c r="C135" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>84</v>
+      </c>
+      <c r="B136">
+        <v>2</v>
+      </c>
+      <c r="C136" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>86</v>
+      </c>
+      <c r="B137">
+        <v>2</v>
+      </c>
+      <c r="C137" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>88</v>
+      </c>
+      <c r="B138">
+        <v>2</v>
+      </c>
+      <c r="C138" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>90</v>
+      </c>
+      <c r="B139">
+        <v>2</v>
+      </c>
+      <c r="C139" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>